<commit_message>
Changing test time file.
</commit_message>
<xml_diff>
--- a/TestTime.xlsx
+++ b/TestTime.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
@@ -469,7 +469,7 @@
         <v>50</v>
       </c>
       <c r="H2">
-        <v>290</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>